<commit_message>
Update files from Google Drive
Commit file that have already update in Google Drive
File lastest at 0:18 Tuesday 27th July 2021
</commit_message>
<xml_diff>
--- a/admin/Example1.xlsx
+++ b/admin/Example1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TTPS\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6727132-D9FE-43C0-BCBD-B1E224E9B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC0CCAB-7EC0-4150-B6CA-D6C0CBD8A07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6390E7E7-2793-4C10-9843-D22A1AFB05B4}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{6390E7E7-2793-4C10-9843-D22A1AFB05B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>ม.4/1</t>
   </si>
   <si>
-    <t>ม.6/1</t>
-  </si>
-  <si>
     <t>อ 11011</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>ค 11012</t>
+  </si>
+  <si>
+    <t>ม.6/2</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1">
         <v>2564</v>
@@ -512,13 +512,13 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -532,10 +532,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -546,13 +546,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -566,10 +566,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -583,10 +583,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -597,13 +597,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
codes from google Drive (lastest: 20210914) I will comment later.
</commit_message>
<xml_diff>
--- a/admin/Example1.xlsx
+++ b/admin/Example1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TTPS\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC0CCAB-7EC0-4150-B6CA-D6C0CBD8A07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC6DEBC-B93D-4916-9A2F-B34926F6BF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" xr2:uid="{6390E7E7-2793-4C10-9843-D22A1AFB05B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6390E7E7-2793-4C10-9843-D22A1AFB05B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,44 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
-  <si>
-    <t>08:00 - 09:00</t>
-  </si>
-  <si>
-    <t>09:00 - 10:00</t>
-  </si>
-  <si>
-    <t>10:00 - 11:00</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>จันทร์</t>
-  </si>
-  <si>
-    <t>อังคาร</t>
-  </si>
-  <si>
-    <t>พุธ</t>
-  </si>
-  <si>
-    <t>พฤหัสบดี</t>
-  </si>
-  <si>
-    <t>ศุกร์</t>
-  </si>
-  <si>
-    <t>นางสาวทดสอบ</t>
-  </si>
-  <si>
     <t>รหัสวิชา</t>
   </si>
   <si>
@@ -81,24 +48,6 @@
     <t>ป.1/1</t>
   </si>
   <si>
-    <t>ม.1/1</t>
-  </si>
-  <si>
-    <t>ม.4/1</t>
-  </si>
-  <si>
-    <t>อ 11011</t>
-  </si>
-  <si>
-    <t>อ 12012</t>
-  </si>
-  <si>
-    <t>ว 21021</t>
-  </si>
-  <si>
-    <t>ว 42002</t>
-  </si>
-  <si>
     <t>ชั้น</t>
   </si>
   <si>
@@ -108,19 +57,19 @@
     <t>ประถมศึกษา</t>
   </si>
   <si>
-    <t>มัธยมศึกษา</t>
-  </si>
-  <si>
-    <t>ป.4/1</t>
-  </si>
-  <si>
     <t>คุณครู</t>
   </si>
   <si>
-    <t>ค 11012</t>
-  </si>
-  <si>
-    <t>ม.6/2</t>
+    <t>ทดสอบ</t>
+  </si>
+  <si>
+    <t>วันพุธ</t>
+  </si>
+  <si>
+    <t>14:00 - 15:00</t>
+  </si>
+  <si>
+    <t>ค 11101</t>
   </si>
 </sst>
 </file>
@@ -478,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EE8E88-F3C7-4D91-AE65-AA1217A6670B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,115 +444,47 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C1">
-        <v>2564</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added codes from v0.4 branch.
    I will comment later.
</commit_message>
<xml_diff>
--- a/admin/Example1.xlsx
+++ b/admin/Example1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TTPS\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6727132-D9FE-43C0-BCBD-B1E224E9B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC6DEBC-B93D-4916-9A2F-B34926F6BF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6390E7E7-2793-4C10-9843-D22A1AFB05B4}"/>
   </bookViews>
@@ -34,44 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
-  <si>
-    <t>08:00 - 09:00</t>
-  </si>
-  <si>
-    <t>09:00 - 10:00</t>
-  </si>
-  <si>
-    <t>10:00 - 11:00</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>จันทร์</t>
-  </si>
-  <si>
-    <t>อังคาร</t>
-  </si>
-  <si>
-    <t>พุธ</t>
-  </si>
-  <si>
-    <t>พฤหัสบดี</t>
-  </si>
-  <si>
-    <t>ศุกร์</t>
-  </si>
-  <si>
-    <t>นางสาวทดสอบ</t>
-  </si>
-  <si>
     <t>รหัสวิชา</t>
   </si>
   <si>
@@ -81,27 +48,6 @@
     <t>ป.1/1</t>
   </si>
   <si>
-    <t>ม.1/1</t>
-  </si>
-  <si>
-    <t>ม.4/1</t>
-  </si>
-  <si>
-    <t>ม.6/1</t>
-  </si>
-  <si>
-    <t>อ 11011</t>
-  </si>
-  <si>
-    <t>อ 12012</t>
-  </si>
-  <si>
-    <t>ว 21021</t>
-  </si>
-  <si>
-    <t>ว 42002</t>
-  </si>
-  <si>
     <t>ชั้น</t>
   </si>
   <si>
@@ -111,16 +57,19 @@
     <t>ประถมศึกษา</t>
   </si>
   <si>
-    <t>มัธยมศึกษา</t>
-  </si>
-  <si>
-    <t>ป.4/1</t>
-  </si>
-  <si>
     <t>คุณครู</t>
   </si>
   <si>
-    <t>ค 11012</t>
+    <t>ทดสอบ</t>
+  </si>
+  <si>
+    <t>วันพุธ</t>
+  </si>
+  <si>
+    <t>14:00 - 15:00</t>
+  </si>
+  <si>
+    <t>ค 11101</t>
   </si>
 </sst>
 </file>
@@ -478,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EE8E88-F3C7-4D91-AE65-AA1217A6670B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,115 +444,47 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C1">
-        <v>2564</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>